<commit_message>
Naujas UC ir Reikalavimu numeravimas
</commit_message>
<xml_diff>
--- a/PSI II Lab 3/UCxFR.xlsx
+++ b/PSI II Lab 3/UCxFR.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomas\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steror\Documents\GitHub\Slidinejimas\PSI II Lab 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5959001-25EA-4B2C-900F-53091F0B674F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9090" xr2:uid="{B89CD281-05C4-4C8B-B7F4-47BC48F0502B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9090"/>
   </bookViews>
   <sheets>
     <sheet name="UCxFR" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <r>
       <rPr>
@@ -74,18 +73,6 @@
     <t>UC 10</t>
   </si>
   <si>
-    <t>UC 11</t>
-  </si>
-  <si>
-    <t>UC 12</t>
-  </si>
-  <si>
-    <t>UC 13</t>
-  </si>
-  <si>
-    <t>UC 14</t>
-  </si>
-  <si>
     <t>FR 1</t>
   </si>
   <si>
@@ -122,26 +109,32 @@
     <t>FR 15</t>
   </si>
   <si>
-    <t>FR 16</t>
-  </si>
-  <si>
-    <t>FR 17</t>
-  </si>
-  <si>
-    <t>FR 19</t>
-  </si>
-  <si>
-    <t>FR 20</t>
-  </si>
-  <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>UC 3</t>
+  </si>
+  <si>
+    <t>UC 5</t>
+  </si>
+  <si>
+    <t>UC 9</t>
+  </si>
+  <si>
+    <t>FR 9</t>
+  </si>
+  <si>
+    <t>FR 12</t>
+  </si>
+  <si>
+    <t>FR 14</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,11 +151,6 @@
       <family val="2"/>
       <charset val="186"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Helvetica"/>
     </font>
   </fonts>
   <fills count="2">
@@ -200,15 +188,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment textRotation="135" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -525,338 +510,302 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDFD0500-70CD-4EB1-84CF-345DDEB1E1DB}">
-  <dimension ref="A1:Q12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="W23" sqref="W23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="17" width="3.7109375" customWidth="1"/>
+    <col min="2" max="16" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="M1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="O1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-    </row>
-    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+    </row>
+    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+    </row>
+    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-    </row>
-    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+    </row>
+    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+    </row>
+    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-    </row>
-    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+    </row>
+    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-    </row>
-    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+    </row>
+    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-    </row>
-    <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+    </row>
+    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P10" s="3"/>
+    </row>
+    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-    </row>
-    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-    </row>
-    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q10" s="4"/>
-    </row>
-    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
-    </row>
-    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
+      <c r="B11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>